<commit_message>
testFormProcessesAsExpected test passes and datetime wrapped in class for mocking
</commit_message>
<xml_diff>
--- a/tests/fixtures/money_out_template.xlsx
+++ b/tests/fixtures/money_out_template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Payment Type</t>
   </si>
@@ -38,15 +38,6 @@
   </si>
   <si>
     <t>Current</t>
-  </si>
-  <si>
-    <t>Rent</t>
-  </si>
-  <si>
-    <t>Moved home</t>
-  </si>
-  <si>
-    <t>Medical Expenses</t>
   </si>
 </sst>
 </file>
@@ -132,7 +123,7 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -300,13 +291,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -396,19 +381,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -663,13 +648,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -973,19 +952,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1293,30 +1272,16 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="4">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5">
-        <v>20000</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s" s="4">
-        <v>10</v>
-      </c>
+      <c r="A4" s="4"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1700</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>8</v>
-      </c>
+      <c r="A5" s="4"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
       <c r="D5" s="6"/>
       <c r="E5" s="3"/>
     </row>
@@ -1637,7 +1602,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A3 A6:A50">
       <formula1>"Care Fees,Clothes,Broadband,Council Tax,Electricity,Food,Rent,Medical Expenses,Mortgage,Personal Allowance,Water,Wifi"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>